<commit_message>
added comment on excel file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Donlon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ethan Donlon\Documents\Documents\Dove Git\AromringFork\MAX30102_by_RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C0F62E-83BD-42F6-BE78-8082C814A03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693D5D36-D566-4700-936C-1DC1F36BED6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30135" yWindow="165" windowWidth="26865" windowHeight="14925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6974,6 +6974,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1054494160"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -7059,6 +7060,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -9233,6 +9235,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15292,6 +15295,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1091478128"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -17053,15 +17057,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>81998</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>65433</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>59427</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>240195</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>149087</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17089,15 +17093,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>431522</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>145979</xdr:rowOff>
+      <xdr:colOff>464652</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>30022</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>82826</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>173934</xdr:rowOff>
+      <xdr:colOff>115956</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>57977</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17126,6 +17130,172 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.1386</cdr:x>
+      <cdr:y>0.10515</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.84689</cdr:x>
+      <cdr:y>0.44243</cdr:y>
+    </cdr:to>
+    <cdr:grpSp>
+      <cdr:nvGrpSpPr>
+        <cdr:cNvPr id="4" name="Group 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{840EA1E4-1C1E-3373-CC3E-2D51E6120360}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvGrpSpPr/>
+      </cdr:nvGrpSpPr>
+      <cdr:grpSpPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="776153" y="344725"/>
+          <a:ext cx="3966314" cy="1105771"/>
+          <a:chOff x="776153" y="344725"/>
+          <a:chExt cx="3966314" cy="1105771"/>
+        </a:xfrm>
+      </cdr:grpSpPr>
+      <cdr:sp macro="" textlink="">
+        <cdr:nvSpPr>
+          <cdr:cNvPr id="2" name="TextBox 1">
+            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{350D4E1C-1809-E83E-EEB4-02C54C101BC9}"/>
+              </a:ext>
+            </a:extLst>
+          </cdr:cNvPr>
+          <cdr:cNvSpPr txBox="1"/>
+        </cdr:nvSpPr>
+        <cdr:spPr>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:off x="776153" y="344725"/>
+            <a:ext cx="1955514" cy="1092821"/>
+          </a:xfrm>
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </cdr:spPr>
+        <cdr:txBody>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Put</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0"/>
+              <a:t> hand on device, it begins to calibrate</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </cdr:txBody>
+      </cdr:sp>
+      <cdr:sp macro="" textlink="">
+        <cdr:nvSpPr>
+          <cdr:cNvPr id="3" name="TextBox 1">
+            <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89CD0D4C-825B-17F5-9B78-70B7DCFEC449}"/>
+              </a:ext>
+            </a:extLst>
+          </cdr:cNvPr>
+          <cdr:cNvSpPr txBox="1"/>
+        </cdr:nvSpPr>
+        <cdr:spPr>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:off x="2786954" y="357674"/>
+            <a:ext cx="1955513" cy="1092822"/>
+          </a:xfrm>
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </cdr:spPr>
+        <cdr:txBody>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:lvl1pPr marL="0" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" indent="0">
+              <a:defRPr sz="1100">
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:r>
+              <a:rPr lang="en-US" sz="1100"/>
+              <a:t>Take hand off, and put hand back on, to see calibrate again</a:t>
+            </a:r>
+          </a:p>
+        </cdr:txBody>
+      </cdr:sp>
+    </cdr:grpSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17454,7 +17624,7 @@
   <dimension ref="A1:D673"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>